<commit_message>
v1.2 add header_row_num parameter to TableReader
update project link

ready for v1.2 release
</commit_message>
<xml_diff>
--- a/tests/test_files/test_utils.xlsx
+++ b/tests/test_files/test_utils.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chuki\projects\openpyxl_utils\tests\test_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\excelerator\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75901944-E5F4-4452-BA39-E574B0FA5DD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14039A4A-2805-498A-ACCA-A85EE14CF473}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10155" yWindow="5550" windowWidth="24510" windowHeight="11910" tabRatio="699" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="699" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentors" sheetId="2" r:id="rId1"/>
@@ -19,8 +19,10 @@
     <sheet name="drop_dups" sheetId="7" r:id="rId4"/>
     <sheet name="test_converters" sheetId="5" r:id="rId5"/>
     <sheet name="worksheet_rows" sheetId="9" r:id="rId6"/>
-    <sheet name="simple_table_left" sheetId="10" r:id="rId7"/>
-    <sheet name="simple_table_right" sheetId="11" r:id="rId8"/>
+    <sheet name="table_top_left" sheetId="10" r:id="rId7"/>
+    <sheet name="table_top_right" sheetId="11" r:id="rId8"/>
+    <sheet name="table_bottom_left" sheetId="12" r:id="rId9"/>
+    <sheet name="table_bottom_right" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="79">
   <si>
     <t>hello</t>
   </si>
@@ -594,10 +596,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74385198-D54E-4AE5-817F-A59CEFD9899A}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,8 +704,73 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C01D03-48FB-4B42-B3DE-BFEE86FD73A2}">
+  <dimension ref="D4:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="6" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2522D482-B94D-46FB-A9F8-A8684FBBFA17}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -820,6 +890,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28ADF7BC-4D61-4B69-9FD5-BB55FF4CFF0C}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -895,6 +968,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2ED103-366B-4811-A01C-B5BA0C05633E}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -970,6 +1046,9 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767763AB-0C65-45CA-B5A2-51B6577CE94A}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1296,6 +1375,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CF0A76-D4B7-4F29-A377-9B2B3E0D669D}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="B4:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1402,7 +1484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783C3457-7CDB-477F-9144-DC6CA0AEA38D}">
   <dimension ref="E1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1458,4 +1540,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326A8A59-3B6E-4818-8D8B-9A673D0EDFC4}">
+  <dimension ref="A4:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C6">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add first 3 norm functions
listofints start wip

ws for testing normalization

test_normalize.py

test written

coded first three norm types

coded TableReader

implement given when then in tests

tests pass

docs wip

add m2r

uprev
</commit_message>
<xml_diff>
--- a/tests/test_files/test_utils.xlsx
+++ b/tests/test_files/test_utils.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchukina\projects\excelerator\tests\test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14039A4A-2805-498A-ACCA-A85EE14CF473}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F55AD1-594A-4DBE-A999-F5C18BA6F19B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="699" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" tabRatio="699" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mentors" sheetId="2" r:id="rId1"/>
     <sheet name="mentees" sheetId="3" r:id="rId2"/>
     <sheet name="test_index_names" sheetId="4" r:id="rId3"/>
     <sheet name="drop_dups" sheetId="7" r:id="rId4"/>
-    <sheet name="test_converters" sheetId="5" r:id="rId5"/>
-    <sheet name="worksheet_rows" sheetId="9" r:id="rId6"/>
-    <sheet name="table_top_left" sheetId="10" r:id="rId7"/>
-    <sheet name="table_top_right" sheetId="11" r:id="rId8"/>
-    <sheet name="table_bottom_left" sheetId="12" r:id="rId9"/>
-    <sheet name="table_bottom_right" sheetId="13" r:id="rId10"/>
+    <sheet name="table_top_left" sheetId="10" r:id="rId5"/>
+    <sheet name="table_top_right" sheetId="11" r:id="rId6"/>
+    <sheet name="table_bottom_left" sheetId="12" r:id="rId7"/>
+    <sheet name="table_bottom_right" sheetId="13" r:id="rId8"/>
+    <sheet name="normalize" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,10 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="79">
-  <si>
-    <t>hello</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
   <si>
     <t>first_name</t>
   </si>
@@ -87,45 +83,18 @@
     <t xml:space="preserve">two spaces right  </t>
   </si>
   <si>
-    <t>appl</t>
-  </si>
-  <si>
-    <t>grapes</t>
-  </si>
-  <si>
-    <t>ap</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>The answer should be 4!</t>
-  </si>
-  <si>
-    <t>string</t>
-  </si>
-  <si>
-    <t>list_of_words</t>
-  </si>
-  <si>
     <t>hello, good bye</t>
   </si>
   <si>
     <t>123 456 78hi</t>
   </si>
   <si>
-    <t>first_digit</t>
-  </si>
-  <si>
     <t>20 manager</t>
   </si>
   <si>
     <t>helper 30</t>
   </si>
   <si>
-    <t>tuple_ints</t>
-  </si>
-  <si>
     <t>1, 2, 3</t>
   </si>
   <si>
@@ -135,30 +104,15 @@
     <t>19twenty3</t>
   </si>
   <si>
-    <t>boolean</t>
-  </si>
-  <si>
-    <t>ints_with_missing</t>
-  </si>
-  <si>
-    <t>all_numbers</t>
-  </si>
-  <si>
     <t>float</t>
   </si>
   <si>
-    <t>first_digit_missing</t>
-  </si>
-  <si>
     <t>30 manager</t>
   </si>
   <si>
     <t>4</t>
   </si>
   <si>
-    <t>boolean_perfect</t>
-  </si>
-  <si>
     <t>I should</t>
   </si>
   <si>
@@ -255,9 +209,6 @@
     <t>123, 234, 345</t>
   </si>
   <si>
-    <t>row</t>
-  </si>
-  <si>
     <t>River</t>
   </si>
   <si>
@@ -277,6 +228,39 @@
   </si>
   <si>
     <t>last_appearance</t>
+  </si>
+  <si>
+    <t>values</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>blank space</t>
+  </si>
+  <si>
+    <t>string with leading white space</t>
+  </si>
+  <si>
+    <t>leading apostrophe to force string</t>
+  </si>
+  <si>
+    <t>excel boolean true</t>
+  </si>
+  <si>
+    <t>excel boolean false</t>
+  </si>
+  <si>
+    <t>stringLettersOnly</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>string with trailing white space</t>
   </si>
 </sst>
 </file>
@@ -601,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -619,48 +603,48 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="L1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="C2">
         <v>123</v>
@@ -668,10 +652,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C3">
         <v>234</v>
@@ -679,10 +663,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C4">
         <v>345</v>
@@ -690,75 +674,13 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>456</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C01D03-48FB-4B42-B3DE-BFEE86FD73A2}">
-  <dimension ref="D4:F7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="6" width="18" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E6" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6">
-        <v>2013</v>
-      </c>
-    </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7">
-        <v>2015</v>
       </c>
     </row>
   </sheetData>
@@ -797,54 +719,54 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="L1" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="N1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>1123</v>
@@ -852,7 +774,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="C3">
         <v>1234</v>
@@ -863,24 +785,24 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>1345</v>
       </c>
       <c r="L4" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C5">
         <v>1456</v>
       </c>
       <c r="L5" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -908,21 +830,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1732524</v>
@@ -930,10 +852,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>432436</v>
@@ -941,10 +863,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4">
         <v>423134</v>
@@ -952,10 +874,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>43243</v>
@@ -986,21 +908,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1732524</v>
@@ -1008,10 +930,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="C3">
         <v>43243</v>
@@ -1019,10 +941,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C4">
         <v>43243</v>
@@ -1030,10 +952,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5">
         <v>423134</v>
@@ -1045,380 +967,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767763AB-0C65-45CA-B5A2-51B6577CE94A}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="A1:J10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="b">
-        <v>0</v>
-      </c>
-      <c r="B3" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>457</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
-      </c>
-      <c r="F3" t="b">
-        <v>0</v>
-      </c>
-      <c r="G3" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" t="b">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>63.5</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" t="b">
-        <v>1</v>
-      </c>
-      <c r="G4" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>465</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>77557357</v>
-      </c>
-      <c r="I6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C7">
-        <v>57</v>
-      </c>
-      <c r="G7" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>12541</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" t="b">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>25.5</v>
-      </c>
-      <c r="I8">
-        <v>25.5</v>
-      </c>
-      <c r="J8">
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>858</v>
-      </c>
-      <c r="I9">
-        <v>858</v>
-      </c>
-      <c r="J9">
-        <v>858</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>43756</v>
-      </c>
-      <c r="B10" s="2">
-        <v>43756</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10" s="2">
-        <v>43756</v>
-      </c>
-      <c r="E10" s="2">
-        <v>43756</v>
-      </c>
-      <c r="F10" s="2">
-        <v>43756</v>
-      </c>
-      <c r="G10" t="b">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>23</v>
-      </c>
-      <c r="I10" s="2">
-        <v>43756</v>
-      </c>
-      <c r="J10" s="2">
-        <v>43756</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CF0A76-D4B7-4F29-A377-9B2B3E0D669D}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
-  <dimension ref="B4:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{262E72F4-25ED-4525-A02C-BF33E868C3A6}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1433,21 +981,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C2">
         <v>2013</v>
@@ -1455,10 +1003,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C3">
         <v>2013</v>
@@ -1466,10 +1014,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C4">
         <v>2015</v>
@@ -1480,7 +1028,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{783C3457-7CDB-477F-9144-DC6CA0AEA38D}">
   <dimension ref="E1:G4"/>
   <sheetViews>
@@ -1495,21 +1043,21 @@
   <sheetData>
     <row r="1" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="G2">
         <v>2013</v>
@@ -1517,10 +1065,10 @@
     </row>
     <row r="3" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="G3">
         <v>2013</v>
@@ -1528,10 +1076,10 @@
     </row>
     <row r="4" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="G4">
         <v>2015</v>
@@ -1542,7 +1090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{326A8A59-3B6E-4818-8D8B-9A673D0EDFC4}">
   <dimension ref="A4:C7"/>
   <sheetViews>
@@ -1557,21 +1105,21 @@
   <sheetData>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="C5">
         <v>2013</v>
@@ -1579,10 +1127,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="C6">
         <v>2013</v>
@@ -1590,10 +1138,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="C7">
         <v>2015</v>
@@ -1602,4 +1150,274 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16C01D03-48FB-4B42-B3DE-BFEE86FD73A2}">
+  <dimension ref="D4:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="6" width="18" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F5">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7">
+        <v>2015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{767763AB-0C65-45CA-B5A2-51B6577CE94A}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>457</v>
+      </c>
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>525.4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>663.5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>663.6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>43756</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="b">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="b">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B26">
+    <sortCondition ref="A26"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>